<commit_message>
PMMA const & linear
</commit_message>
<xml_diff>
--- a/Properties.xlsx
+++ b/Properties.xlsx
@@ -84,7 +84,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -114,7 +114,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0F0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -181,8 +187,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -195,14 +210,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,7 +496,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,514 +510,514 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="8">
         <v>50800000000</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <f>B3*0.8</f>
         <v>40640000000</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="1">
         <f>B3*1.2</f>
         <v>60960000000</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="1">
         <f>B3/4</f>
         <v>12700000000</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="1">
         <f>B3*4</f>
         <v>203200000000</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="8">
         <v>50800000000</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="1">
         <f>G3*0.8</f>
         <v>40640000000</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="1">
         <f>G3*1.2</f>
         <v>60960000000</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="3">
         <f>G3/4</f>
         <v>12700000000</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="3">
         <f>G3*4</f>
         <v>203200000000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="8">
         <v>157000</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <f t="shared" ref="C4:C13" si="0">B4*0.8</f>
         <v>125600</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="1">
         <f t="shared" ref="D4:D13" si="1">B4*1.2</f>
         <v>188400</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="1">
         <f t="shared" ref="E4:E13" si="2">B4/4</f>
         <v>39250</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="1">
         <f t="shared" ref="F4:F13" si="3">B4*4</f>
         <v>628000</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="8">
         <v>157000</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="1">
         <f t="shared" ref="H4:H13" si="4">G4*0.8</f>
         <v>125600</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="1">
         <f t="shared" ref="I4:I13" si="5">G4*1.2</f>
         <v>188400</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="3">
         <f t="shared" ref="J4:J13" si="6">G4/4</f>
         <v>39250</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="3">
         <f t="shared" ref="K4:K13" si="7">G4*4</f>
         <v>628000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="8">
         <v>0.91</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>0.72800000000000009</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
         <v>1.0920000000000001</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="1">
         <f t="shared" si="2"/>
         <v>0.22750000000000001</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="1">
         <f t="shared" si="3"/>
         <v>3.64</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="8">
         <v>0.91</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="1">
         <f t="shared" si="4"/>
         <v>0.72800000000000009</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="1">
         <f t="shared" si="5"/>
         <v>1.0920000000000001</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="3">
         <f t="shared" si="6"/>
         <v>0.22750000000000001</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="3">
         <f t="shared" si="7"/>
         <v>3.64</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="8">
         <v>788000</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>630400</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
         <v>945600</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="1">
         <f t="shared" si="2"/>
         <v>197000</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="1">
         <f t="shared" si="3"/>
         <v>3152000</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="8">
         <v>788000</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="1">
         <f t="shared" si="4"/>
         <v>630400</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="1">
         <f t="shared" si="5"/>
         <v>945600</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="3">
         <f t="shared" si="6"/>
         <v>197000</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="3">
         <f t="shared" si="7"/>
         <v>3152000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="8">
         <v>0.249</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>0.19920000000000002</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="1">
         <f t="shared" si="1"/>
         <v>0.29880000000000001</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
         <v>6.225E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="1">
         <f t="shared" si="3"/>
         <v>0.996</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="8">
         <v>0.21</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="1">
         <f t="shared" si="4"/>
         <v>0.16800000000000001</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="1">
         <f t="shared" si="5"/>
         <v>0.252</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="3">
         <f t="shared" si="6"/>
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="3">
         <f t="shared" si="7"/>
         <v>0.84</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="8">
         <v>0</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="8">
         <v>2.5999999999999998E-4</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="1">
         <f t="shared" si="4"/>
         <v>2.0799999999999999E-4</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="1">
         <f t="shared" si="5"/>
         <v>3.1199999999999994E-4</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="3">
         <f t="shared" si="6"/>
         <v>6.4999999999999994E-5</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="3">
         <f t="shared" si="7"/>
         <v>1.0399999999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="8">
         <v>1886</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>1508.8000000000002</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>2263.1999999999998</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
         <v>471.5</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="1">
         <f t="shared" si="3"/>
         <v>7544</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="8">
         <v>1289.2</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="1">
         <f t="shared" si="4"/>
         <v>1031.3600000000001</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="1">
         <f t="shared" si="5"/>
         <v>1547.04</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="3">
         <f t="shared" si="6"/>
         <v>322.3</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="3">
         <f t="shared" si="7"/>
         <v>5156.8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="8">
         <v>0</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="8">
         <v>3.9779</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="1">
         <f t="shared" si="4"/>
         <v>3.1823200000000003</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="1">
         <f t="shared" si="5"/>
         <v>4.7734800000000002</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="3">
         <f t="shared" si="6"/>
         <v>0.994475</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="3">
         <f t="shared" si="7"/>
         <v>15.9116</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="8">
         <v>1189.3699999999999</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="8">
         <v>1189.3699999999999</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="8">
         <v>0.8</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>0.64000000000000012</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>0.96</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="1">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="1">
         <f t="shared" si="3"/>
         <v>3.2</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="8">
         <v>0.8</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="1">
         <f t="shared" si="4"/>
         <v>0.64000000000000012</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="1">
         <f t="shared" si="5"/>
         <v>0.96</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="3">
         <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="3">
         <f t="shared" si="7"/>
         <v>3.2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="8">
         <v>1000</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="1">
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="1">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="8">
         <v>1000</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="1">
         <f t="shared" si="4"/>
         <v>800</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="1">
         <f t="shared" si="5"/>
         <v>1200</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="3">
         <f t="shared" si="6"/>
         <v>250</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="3">
         <f t="shared" si="7"/>
         <v>4000</v>
       </c>

</xml_diff>

<commit_message>
Making E_Glass constant case, fix PMMA cases
</commit_message>
<xml_diff>
--- a/Properties.xlsx
+++ b/Properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PMMA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>Input parameters</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>Target value (Linear)</t>
+  </si>
+  <si>
+    <t>kc_a (W/m/K)</t>
+  </si>
+  <si>
+    <t>kc_b (W/m/K^2)</t>
+  </si>
+  <si>
+    <t>Cpc_a (J/kg/K)</t>
+  </si>
+  <si>
+    <t>Cpc_b (J/kg/K^2)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -197,6 +209,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -210,8 +225,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,58 +528,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>50800000000</v>
       </c>
       <c r="C3" s="1">
@@ -580,7 +598,7 @@
         <f>B3*4</f>
         <v>203200000000</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="4">
         <v>50800000000</v>
       </c>
       <c r="H3" s="1">
@@ -604,7 +622,7 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>157000</v>
       </c>
       <c r="C4" s="1">
@@ -623,7 +641,7 @@
         <f t="shared" ref="F4:F13" si="3">B4*4</f>
         <v>628000</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="4">
         <v>157000</v>
       </c>
       <c r="H4" s="1">
@@ -647,7 +665,7 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>0.91</v>
       </c>
       <c r="C5" s="1">
@@ -666,7 +684,7 @@
         <f t="shared" si="3"/>
         <v>3.64</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="4">
         <v>0.91</v>
       </c>
       <c r="H5" s="1">
@@ -690,7 +708,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>788000</v>
       </c>
       <c r="C6" s="1">
@@ -709,7 +727,7 @@
         <f t="shared" si="3"/>
         <v>3152000</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="4">
         <v>788000</v>
       </c>
       <c r="H6" s="1">
@@ -733,7 +751,7 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>0.249</v>
       </c>
       <c r="C7" s="1">
@@ -752,7 +770,7 @@
         <f t="shared" si="3"/>
         <v>0.996</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="4">
         <v>0.21</v>
       </c>
       <c r="H7" s="1">
@@ -776,7 +794,7 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>0</v>
       </c>
       <c r="C8" s="1">
@@ -795,7 +813,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="4">
         <v>2.5999999999999998E-4</v>
       </c>
       <c r="H8" s="1">
@@ -819,7 +837,7 @@
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="4">
         <v>1886</v>
       </c>
       <c r="C9" s="1">
@@ -838,7 +856,7 @@
         <f t="shared" si="3"/>
         <v>7544</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="4">
         <v>1289.2</v>
       </c>
       <c r="H9" s="1">
@@ -862,7 +880,7 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="4">
         <v>0</v>
       </c>
       <c r="C10" s="1">
@@ -881,7 +899,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="4">
         <v>3.9779</v>
       </c>
       <c r="H10" s="1">
@@ -905,7 +923,7 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>1189.3699999999999</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -920,7 +938,7 @@
       <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="4">
         <v>1189.3699999999999</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -940,7 +958,7 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="4">
         <v>0.8</v>
       </c>
       <c r="C12" s="1">
@@ -959,7 +977,7 @@
         <f t="shared" si="3"/>
         <v>3.2</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="4">
         <v>0.8</v>
       </c>
       <c r="H12" s="1">
@@ -983,7 +1001,7 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="4">
         <v>1000</v>
       </c>
       <c r="C13" s="1">
@@ -1002,7 +1020,7 @@
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="4">
         <v>1000</v>
       </c>
       <c r="H13" s="1">
@@ -1043,14 +1061,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
E-glass linear optimization cases
</commit_message>
<xml_diff>
--- a/Properties.xlsx
+++ b/Properties.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>Input parameters</t>
   </si>
@@ -89,14 +89,24 @@
   </si>
   <si>
     <t>Cpc_b (J/kg/K^2)</t>
+  </si>
+  <si>
+    <t>ρc (kg/m^3)</t>
+  </si>
+  <si>
+    <t>εc</t>
+  </si>
+  <si>
+    <t>Kv (1/m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -199,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -214,6 +224,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -225,12 +241,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +527,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,52 +541,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1061,53 +1074,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1115,78 +1125,731 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="12">
+        <v>3380000000000000</v>
+      </c>
+      <c r="C2" s="11">
+        <f>B2*0.8</f>
+        <v>2704000000000000</v>
+      </c>
+      <c r="D2" s="11">
+        <f>B2*1.2</f>
+        <v>4056000000000000</v>
+      </c>
+      <c r="E2" s="11">
+        <f>B2/4</f>
+        <v>845000000000000</v>
+      </c>
+      <c r="F2" s="11">
+        <f>B2*4</f>
+        <v>1.352E+16</v>
+      </c>
+      <c r="G2" s="12">
+        <v>3380000000000000</v>
+      </c>
+      <c r="H2" s="11">
+        <f>G2*0.8</f>
+        <v>2704000000000000</v>
+      </c>
+      <c r="I2" s="11">
+        <f>G2*1.2</f>
+        <v>4056000000000000</v>
+      </c>
+      <c r="J2" s="11">
+        <f>G2/4</f>
+        <v>845000000000000</v>
+      </c>
+      <c r="K2" s="11">
+        <f>G2*4</f>
+        <v>1.352E+16</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="12">
+        <v>213000</v>
+      </c>
+      <c r="C3" s="11">
+        <f t="shared" ref="C3:C18" si="0">B3*0.8</f>
+        <v>170400</v>
+      </c>
+      <c r="D3" s="11">
+        <f t="shared" ref="D3:D18" si="1">B3*1.2</f>
+        <v>255600</v>
+      </c>
+      <c r="E3" s="11">
+        <f t="shared" ref="E3:E18" si="2">B3/4</f>
+        <v>53250</v>
+      </c>
+      <c r="F3" s="11">
+        <f t="shared" ref="F3:F18" si="3">B3*4</f>
+        <v>852000</v>
+      </c>
+      <c r="G3" s="12">
+        <v>213000</v>
+      </c>
+      <c r="H3" s="11">
+        <f t="shared" ref="H3:H18" si="4">G3*0.8</f>
+        <v>170400</v>
+      </c>
+      <c r="I3" s="11">
+        <f t="shared" ref="I3:I18" si="5">G3*1.2</f>
+        <v>255600</v>
+      </c>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J18" si="6">G3/4</f>
+        <v>53250</v>
+      </c>
+      <c r="K3" s="11">
+        <f t="shared" ref="K3:K18" si="7">G3*4</f>
+        <v>852000</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="11">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="D4" s="11">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E4" s="11">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G4" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="4"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="I4" s="11">
+        <f t="shared" si="5"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="J4" s="11">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="K4" s="11">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="12">
+        <v>595000</v>
+      </c>
+      <c r="C5" s="11">
+        <f t="shared" si="0"/>
+        <v>476000</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="1"/>
+        <v>714000</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="2"/>
+        <v>148750</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="3"/>
+        <v>2380000</v>
+      </c>
+      <c r="G5" s="12">
+        <v>595000</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="4"/>
+        <v>476000</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="5"/>
+        <v>714000</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="6"/>
+        <v>148750</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="7"/>
+        <v>2380000</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.312</v>
+      </c>
+      <c r="H6" s="11">
+        <f t="shared" si="4"/>
+        <v>0.24960000000000002</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" si="5"/>
+        <v>0.37440000000000001</v>
+      </c>
+      <c r="J6" s="11">
+        <f t="shared" si="6"/>
+        <v>7.8E-2</v>
+      </c>
+      <c r="K6" s="11">
+        <f t="shared" si="7"/>
+        <v>1.248</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="13">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>4.405E-5</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="4"/>
+        <v>3.5240000000000001E-5</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="5"/>
+        <v>5.2859999999999999E-5</v>
+      </c>
+      <c r="J7" s="11">
+        <f t="shared" si="6"/>
+        <v>1.10125E-5</v>
+      </c>
+      <c r="K7" s="11">
+        <f t="shared" si="7"/>
+        <v>1.762E-4</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="13">
+        <v>1090</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="0"/>
+        <v>872</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="1"/>
+        <v>1308</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="2"/>
+        <v>272.5</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="3"/>
+        <v>4360</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1080</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="4"/>
+        <v>864</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="5"/>
+        <v>1296</v>
+      </c>
+      <c r="J8" s="11">
+        <f t="shared" si="6"/>
+        <v>270</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" si="7"/>
+        <v>4320</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="4"/>
+        <v>3.6159999999999998E-2</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="5"/>
+        <v>5.4239999999999997E-2</v>
+      </c>
+      <c r="J9" s="11">
+        <f t="shared" si="6"/>
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" si="7"/>
+        <v>0.18079999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B10" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="0"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="12">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="4"/>
+        <v>7.5920000000000001E-2</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="5"/>
+        <v>0.11388</v>
+      </c>
+      <c r="J10" s="11">
+        <f t="shared" si="6"/>
+        <v>2.3725E-2</v>
+      </c>
+      <c r="K10" s="11">
+        <f t="shared" si="7"/>
+        <v>0.37959999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B11" s="13">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="13">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="4"/>
+        <v>2.264E-4</v>
+      </c>
+      <c r="I11" s="11">
+        <f t="shared" si="5"/>
+        <v>3.3959999999999996E-4</v>
+      </c>
+      <c r="J11" s="11">
+        <f t="shared" si="6"/>
+        <v>7.0749999999999999E-5</v>
+      </c>
+      <c r="K11" s="11">
+        <f t="shared" si="7"/>
+        <v>1.132E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B12" s="12">
+        <v>1150</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" si="0"/>
+        <v>920</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="1"/>
+        <v>1380</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="2"/>
+        <v>287.5</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="3"/>
+        <v>4600</v>
+      </c>
+      <c r="G12" s="12">
+        <v>1041</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="4"/>
+        <v>832.80000000000007</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" si="5"/>
+        <v>1249.2</v>
+      </c>
+      <c r="J12" s="11">
+        <f t="shared" si="6"/>
+        <v>260.25</v>
+      </c>
+      <c r="K12" s="11">
+        <f t="shared" si="7"/>
+        <v>4164</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B13" s="13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="4"/>
+        <v>0.20720000000000002</v>
+      </c>
+      <c r="I13" s="11">
+        <f t="shared" si="5"/>
+        <v>0.31080000000000002</v>
+      </c>
+      <c r="J13" s="11">
+        <f t="shared" si="6"/>
+        <v>6.4750000000000002E-2</v>
+      </c>
+      <c r="K13" s="11">
+        <f t="shared" si="7"/>
+        <v>1.036</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B14" s="12">
+        <v>1683</v>
+      </c>
+      <c r="C14" s="11">
+        <f t="shared" si="0"/>
+        <v>1346.4</v>
+      </c>
+      <c r="D14" s="11">
+        <f t="shared" si="1"/>
+        <v>2019.6</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" si="2"/>
+        <v>420.75</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="3"/>
+        <v>6732</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1683</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="4"/>
+        <v>1346.4</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" si="5"/>
+        <v>2019.6</v>
+      </c>
+      <c r="J14" s="11">
+        <f t="shared" si="6"/>
+        <v>420.75</v>
+      </c>
+      <c r="K14" s="11">
+        <f t="shared" si="7"/>
+        <v>6732</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="12">
+        <v>1235</v>
+      </c>
+      <c r="C15" s="11">
+        <f t="shared" si="0"/>
+        <v>988</v>
+      </c>
+      <c r="D15" s="11">
+        <f t="shared" si="1"/>
+        <v>1482</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="2"/>
+        <v>308.75</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="3"/>
+        <v>4940</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1235</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="4"/>
+        <v>988</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="5"/>
+        <v>1482</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="6"/>
+        <v>308.75</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="7"/>
+        <v>4940</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="2"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="4"/>
+        <v>0.752</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="5"/>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="J16" s="11">
+        <f t="shared" si="6"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="K16" s="11">
+        <f t="shared" si="7"/>
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+      <c r="D17" s="11">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="2"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="4"/>
+        <v>0.752</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="5"/>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="J17" s="11">
+        <f t="shared" si="6"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="7"/>
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="12">
+        <v>10000</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="D18" s="11">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="G18" s="12">
+        <v>10000</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="4"/>
+        <v>8000</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" si="5"/>
+        <v>12000</v>
+      </c>
+      <c r="J18" s="11">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="K18" s="11">
+        <f t="shared" si="7"/>
+        <v>40000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Old linear hybrid run
</commit_message>
<xml_diff>
--- a/Properties.xlsx
+++ b/Properties.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PMMA" sheetId="1" r:id="rId1"/>
     <sheet name="E_Glass" sheetId="2" r:id="rId2"/>
+    <sheet name="E_Glass_Old" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="26">
   <si>
     <t>Input parameters</t>
   </si>
@@ -229,6 +230,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -241,9 +245,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,52 +542,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1076,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,41 +1126,41 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="8">
         <v>3380000000000000</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="7">
         <f>B2*0.8</f>
         <v>2704000000000000</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="7">
         <f>B2*1.2</f>
         <v>4056000000000000</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="7">
         <f>B2/4</f>
         <v>845000000000000</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="7">
         <f>B2*4</f>
         <v>1.352E+16</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="8">
         <v>3380000000000000</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="7">
         <f>G2*0.8</f>
         <v>2704000000000000</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="7">
         <f>G2*1.2</f>
         <v>4056000000000000</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="7">
         <f>G2/4</f>
         <v>845000000000000</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="7">
         <f>G2*4</f>
         <v>1.352E+16</v>
       </c>
@@ -1168,41 +1169,41 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="8">
         <v>213000</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="7">
         <f t="shared" ref="C3:C18" si="0">B3*0.8</f>
         <v>170400</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="7">
         <f t="shared" ref="D3:D18" si="1">B3*1.2</f>
         <v>255600</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="7">
         <f t="shared" ref="E3:E18" si="2">B3/4</f>
         <v>53250</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="7">
         <f t="shared" ref="F3:F18" si="3">B3*4</f>
         <v>852000</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="8">
         <v>213000</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="7">
         <f t="shared" ref="H3:H18" si="4">G3*0.8</f>
         <v>170400</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="7">
         <f t="shared" ref="I3:I18" si="5">G3*1.2</f>
         <v>255600</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="7">
         <f t="shared" ref="J3:J18" si="6">G3/4</f>
         <v>53250</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="7">
         <f t="shared" ref="K3:K18" si="7">G3*4</f>
         <v>852000</v>
       </c>
@@ -1211,41 +1212,41 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="8">
         <v>1.5</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="7">
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="7">
         <f t="shared" si="1"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="7">
         <f t="shared" si="2"/>
         <v>0.375</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="7">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="8">
         <v>1.5</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="7">
         <f t="shared" si="4"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="7">
         <f t="shared" si="5"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="7">
         <f t="shared" si="6"/>
         <v>0.375</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="7">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
@@ -1254,41 +1255,41 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="8">
         <v>595000</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="7">
         <f t="shared" si="0"/>
         <v>476000</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="7">
         <f t="shared" si="1"/>
         <v>714000</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="7">
         <f t="shared" si="2"/>
         <v>148750</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="7">
         <f t="shared" si="3"/>
         <v>2380000</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="8">
         <v>595000</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="7">
         <f t="shared" si="4"/>
         <v>476000</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="7">
         <f t="shared" si="5"/>
         <v>714000</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="7">
         <f t="shared" si="6"/>
         <v>148750</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="7">
         <f t="shared" si="7"/>
         <v>2380000</v>
       </c>
@@ -1297,41 +1298,41 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="9">
         <v>0.3</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="7">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="7">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="7">
         <f t="shared" si="2"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="7">
         <f t="shared" si="3"/>
         <v>1.2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="9">
         <v>0.312</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="7">
         <f t="shared" si="4"/>
         <v>0.24960000000000002</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="7">
         <f t="shared" si="5"/>
         <v>0.37440000000000001</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="7">
         <f t="shared" si="6"/>
         <v>7.8E-2</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="7">
         <f t="shared" si="7"/>
         <v>1.248</v>
       </c>
@@ -1340,41 +1341,41 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13">
-        <v>0</v>
-      </c>
-      <c r="C7" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
         <v>4.405E-5</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="7">
         <f t="shared" si="4"/>
         <v>3.5240000000000001E-5</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="7">
         <f t="shared" si="5"/>
         <v>5.2859999999999999E-5</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="7">
         <f t="shared" si="6"/>
         <v>1.10125E-5</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="7">
         <f t="shared" si="7"/>
         <v>1.762E-4</v>
       </c>
@@ -1383,41 +1384,41 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="9">
         <v>1090</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="7">
         <f t="shared" si="0"/>
         <v>872</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="7">
         <f t="shared" si="1"/>
         <v>1308</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="7">
         <f t="shared" si="2"/>
         <v>272.5</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="7">
         <f t="shared" si="3"/>
         <v>4360</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="9">
         <v>1080</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="7">
         <f t="shared" si="4"/>
         <v>864</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="7">
         <f t="shared" si="5"/>
         <v>1296</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="7">
         <f t="shared" si="6"/>
         <v>270</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="7">
         <f t="shared" si="7"/>
         <v>4320</v>
       </c>
@@ -1426,41 +1427,41 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="13">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="7">
         <f t="shared" si="4"/>
         <v>3.6159999999999998E-2</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="7">
         <f t="shared" si="5"/>
         <v>5.4239999999999997E-2</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="7">
         <f t="shared" si="6"/>
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="7">
         <f t="shared" si="7"/>
         <v>0.18079999999999999</v>
       </c>
@@ -1469,41 +1470,41 @@
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="8">
         <v>0.2</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="7">
         <f t="shared" si="0"/>
         <v>0.16000000000000003</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="7">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="7">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="7">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="8">
         <v>9.4899999999999998E-2</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="7">
         <f t="shared" si="4"/>
         <v>7.5920000000000001E-2</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="7">
         <f t="shared" si="5"/>
         <v>0.11388</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="7">
         <f t="shared" si="6"/>
         <v>2.3725E-2</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="7">
         <f t="shared" si="7"/>
         <v>0.37959999999999999</v>
       </c>
@@ -1512,41 +1513,41 @@
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="13">
-        <v>0</v>
-      </c>
-      <c r="C11" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="13">
+      <c r="B11" s="9">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
         <v>2.8299999999999999E-4</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="7">
         <f t="shared" si="4"/>
         <v>2.264E-4</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="7">
         <f t="shared" si="5"/>
         <v>3.3959999999999996E-4</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="7">
         <f t="shared" si="6"/>
         <v>7.0749999999999999E-5</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="7">
         <f t="shared" si="7"/>
         <v>1.132E-3</v>
       </c>
@@ -1555,41 +1556,41 @@
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="8">
         <v>1150</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="7">
         <f t="shared" si="0"/>
         <v>920</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="7">
         <f t="shared" si="1"/>
         <v>1380</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="7">
         <f t="shared" si="2"/>
         <v>287.5</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="7">
         <f t="shared" si="3"/>
         <v>4600</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="8">
         <v>1041</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="7">
         <f t="shared" si="4"/>
         <v>832.80000000000007</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="7">
         <f t="shared" si="5"/>
         <v>1249.2</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="7">
         <f t="shared" si="6"/>
         <v>260.25</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="7">
         <f t="shared" si="7"/>
         <v>4164</v>
       </c>
@@ -1598,41 +1599,41 @@
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="13">
-        <v>0</v>
-      </c>
-      <c r="C13" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="13">
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
         <v>0.25900000000000001</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="7">
         <f t="shared" si="4"/>
         <v>0.20720000000000002</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="7">
         <f t="shared" si="5"/>
         <v>0.31080000000000002</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="7">
         <f t="shared" si="6"/>
         <v>6.4750000000000002E-2</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="7">
         <f t="shared" si="7"/>
         <v>1.036</v>
       </c>
@@ -1641,41 +1642,41 @@
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="8">
         <v>1683</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>1346.4</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="7">
         <f t="shared" si="1"/>
         <v>2019.6</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="7">
         <f t="shared" si="2"/>
         <v>420.75</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="7">
         <f t="shared" si="3"/>
         <v>6732</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="8">
         <v>1683</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="7">
         <f t="shared" si="4"/>
         <v>1346.4</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="7">
         <f t="shared" si="5"/>
         <v>2019.6</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="7">
         <f t="shared" si="6"/>
         <v>420.75</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="7">
         <f t="shared" si="7"/>
         <v>6732</v>
       </c>
@@ -1684,41 +1685,41 @@
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="8">
         <v>1235</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>988</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="7">
         <f t="shared" si="1"/>
         <v>1482</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="7">
         <f t="shared" si="2"/>
         <v>308.75</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="7">
         <f t="shared" si="3"/>
         <v>4940</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="8">
         <v>1235</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="7">
         <f t="shared" si="4"/>
         <v>988</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="7">
         <f t="shared" si="5"/>
         <v>1482</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="7">
         <f t="shared" si="6"/>
         <v>308.75</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="7">
         <f t="shared" si="7"/>
         <v>4940</v>
       </c>
@@ -1727,39 +1728,39 @@
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="8">
         <v>0.94</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>0.752</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="7">
         <f t="shared" si="2"/>
         <v>0.23499999999999999</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="8">
         <v>0.94</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="7">
         <f t="shared" si="4"/>
         <v>0.752</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="7">
         <f t="shared" si="5"/>
         <v>1.1279999999999999</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="7">
         <f t="shared" si="6"/>
         <v>0.23499999999999999</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="7">
         <f t="shared" si="7"/>
         <v>3.76</v>
       </c>
@@ -1768,39 +1769,39 @@
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="8">
         <v>0.94</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>0.752</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="7">
         <v>1</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="7">
         <f t="shared" si="2"/>
         <v>0.23499999999999999</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="8">
         <v>0.94</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="7">
         <f t="shared" si="4"/>
         <v>0.752</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="7">
         <f t="shared" si="5"/>
         <v>1.1279999999999999</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="7">
         <f t="shared" si="6"/>
         <v>0.23499999999999999</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="7">
         <f t="shared" si="7"/>
         <v>3.76</v>
       </c>
@@ -1809,41 +1810,827 @@
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="8">
         <v>10000</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="7">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="7">
         <f t="shared" si="1"/>
         <v>12000</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="7">
         <f t="shared" si="2"/>
         <v>2500</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="7">
         <f t="shared" si="3"/>
         <v>40000</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="8">
         <v>10000</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="7">
         <f t="shared" si="4"/>
         <v>8000</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="7">
         <f t="shared" si="5"/>
         <v>12000</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="7">
         <f t="shared" si="6"/>
         <v>2500</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="7">
+        <f t="shared" si="7"/>
+        <v>40000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2344000000000</v>
+      </c>
+      <c r="C2" s="7">
+        <f>B2*0.8</f>
+        <v>1875200000000</v>
+      </c>
+      <c r="D2" s="7">
+        <f>B2*1.2</f>
+        <v>2812800000000</v>
+      </c>
+      <c r="E2" s="7">
+        <f>B2/4</f>
+        <v>586000000000</v>
+      </c>
+      <c r="F2" s="7">
+        <f>B2*4</f>
+        <v>9376000000000</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2344000000000</v>
+      </c>
+      <c r="H2" s="7">
+        <f>G2*0.8</f>
+        <v>1875200000000</v>
+      </c>
+      <c r="I2" s="7">
+        <f>G2*1.2</f>
+        <v>2812800000000</v>
+      </c>
+      <c r="J2" s="7">
+        <f>G2/4</f>
+        <v>586000000000</v>
+      </c>
+      <c r="K2" s="7">
+        <f>G2*4</f>
+        <v>9376000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>181000</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C18" si="0">B3*0.8</f>
+        <v>144800</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D18" si="1">B3*1.2</f>
+        <v>217200</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E18" si="2">B3/4</f>
+        <v>45250</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F18" si="3">B3*4</f>
+        <v>724000</v>
+      </c>
+      <c r="G3" s="8">
+        <v>181000</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H18" si="4">G3*0.8</f>
+        <v>144800</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I18" si="5">G3*1.2</f>
+        <v>217200</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J18" si="6">G3/4</f>
+        <v>45250</v>
+      </c>
+      <c r="K3" s="7">
+        <f t="shared" ref="K3:K18" si="7">G3*4</f>
+        <v>724000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="5"/>
+        <v>1.2</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>100000</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="2"/>
+        <v>25000</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="3"/>
+        <v>400000</v>
+      </c>
+      <c r="G5" s="8">
+        <v>100000</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="4"/>
+        <v>80000</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="5"/>
+        <v>120000</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="6"/>
+        <v>25000</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="7"/>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.312</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="4"/>
+        <v>0.24960000000000002</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="5"/>
+        <v>0.37440000000000001</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="6"/>
+        <v>7.8E-2</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="7"/>
+        <v>1.248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>4.405E-5</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="4"/>
+        <v>3.5240000000000001E-5</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="5"/>
+        <v>5.2859999999999999E-5</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="6"/>
+        <v>1.10125E-5</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="7"/>
+        <v>1.762E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1500</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="2"/>
+        <v>375</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>6000</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1080</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="4"/>
+        <v>864</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="5"/>
+        <v>1296</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="6"/>
+        <v>270</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="7"/>
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="4"/>
+        <v>3.6159999999999998E-2</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="5"/>
+        <v>5.4239999999999997E-2</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="6"/>
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="7"/>
+        <v>0.18079999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="8">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="4"/>
+        <v>7.5920000000000001E-2</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="5"/>
+        <v>0.11388</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="6"/>
+        <v>2.3725E-2</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="7"/>
+        <v>0.37959999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="4"/>
+        <v>2.264E-4</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="5"/>
+        <v>3.3959999999999996E-4</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="6"/>
+        <v>7.0749999999999999E-5</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="7"/>
+        <v>1.132E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1100</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>880</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
+        <v>1320</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="2"/>
+        <v>275</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>4400</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1041</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="4"/>
+        <v>832.80000000000007</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="5"/>
+        <v>1249.2</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="6"/>
+        <v>260.25</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="7"/>
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="4"/>
+        <v>0.20720000000000002</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="5"/>
+        <v>0.31080000000000002</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="6"/>
+        <v>6.4750000000000002E-2</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="7"/>
+        <v>1.036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1683</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>1346.4</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
+        <v>2019.6</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="2"/>
+        <v>420.75</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="3"/>
+        <v>6732</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1683</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="4"/>
+        <v>1346.4</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="5"/>
+        <v>2019.6</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="6"/>
+        <v>420.75</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="7"/>
+        <v>6732</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1235</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>988</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
+        <v>1482</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="2"/>
+        <v>308.75</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="3"/>
+        <v>4940</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1235</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="4"/>
+        <v>988</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="5"/>
+        <v>1482</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="6"/>
+        <v>308.75</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="7"/>
+        <v>4940</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="3"/>
+        <v>3.76</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="4"/>
+        <v>0.752</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="5"/>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="6"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="7"/>
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="2"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="3"/>
+        <v>3.76</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="4"/>
+        <v>0.752</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="5"/>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="6"/>
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="7"/>
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="8">
+        <v>10000</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+      <c r="F18" s="7">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+      <c r="G18" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="4"/>
+        <v>8000</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="5"/>
+        <v>12000</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="K18" s="7">
         <f t="shared" si="7"/>
         <v>40000</v>
       </c>

</xml_diff>